<commit_message>
Agrega % de poblacion total y PEA
</commit_message>
<xml_diff>
--- a/data/indicadores_empleo.xlsx
+++ b/data/indicadores_empleo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,50 +446,60 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Poblacion Total (%)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>PEA</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>PEA (%)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Edad PEA</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Desocupacion(%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Informalidad(%)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Desempleo</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Desem ES</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Desem ES(%)</t>
-        </is>
-      </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Desempleo ES</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Desempleo ES(%)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Primario(%)</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Secundario(%)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Terciario(%)</t>
         </is>
@@ -505,33 +515,39 @@
         <v>1473007</v>
       </c>
       <c r="C2" t="n">
+        <v>1.143127762739644</v>
+      </c>
+      <c r="D2" t="n">
         <v>663401</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
+        <v>1.102994380822385</v>
+      </c>
+      <c r="F2" t="n">
         <v>38.343243</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>3.7676</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>40.4789</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>24994</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>14277</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>57.12170921021045</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>4.688545081742525</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>31.13029775676018</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>63.76230210508344</v>
       </c>
     </row>
@@ -545,33 +561,39 @@
         <v>3797115</v>
       </c>
       <c r="C3" t="n">
+        <v>2.946752849657296</v>
+      </c>
+      <c r="D3" t="n">
         <v>1848093</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
+        <v>3.072705941409771</v>
+      </c>
+      <c r="F3" t="n">
         <v>38.846966</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>2.7022</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>36.6282</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>49940</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>24359</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>48.77653183820584</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>2.88785214606321</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>32.14248175767023</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>59.77605910064383</v>
       </c>
     </row>
@@ -585,33 +607,39 @@
         <v>836796</v>
       </c>
       <c r="C4" t="n">
+        <v>0.649395922320453</v>
+      </c>
+      <c r="D4" t="n">
         <v>444018</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
+        <v>0.738240308627804</v>
+      </c>
+      <c r="F4" t="n">
         <v>39.005795</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>2.8508</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>39.3949</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>12658</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>6937</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>54.80328645915626</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>5.824601261127596</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>20.2807399851632</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>73.74374072700297</v>
       </c>
     </row>
@@ -625,33 +653,39 @@
         <v>940944</v>
       </c>
       <c r="C5" t="n">
+        <v>0.7302200258269594</v>
+      </c>
+      <c r="D5" t="n">
         <v>435183</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
+        <v>0.7235509196239197</v>
+      </c>
+      <c r="F5" t="n">
         <v>39.534434</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
         <v>1.9764</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>60.7515</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>8601</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>6078</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>70.66620160446459</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
         <v>18.39904168483433</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>18.96821713058685</v>
       </c>
-      <c r="L5" t="n">
+      <c r="N5" t="n">
         <v>62.23141154572861</v>
       </c>
     </row>
@@ -665,33 +699,39 @@
         <v>5679349</v>
       </c>
       <c r="C6" t="n">
+        <v>4.407461414771034</v>
+      </c>
+      <c r="D6" t="n">
         <v>2211107</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
+        <v>3.676266084008075</v>
+      </c>
+      <c r="F6" t="n">
         <v>39.414684</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
         <v>2.327</v>
       </c>
-      <c r="F6" t="n">
+      <c r="H6" t="n">
         <v>75.1913</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>51452</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>30156</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>58.60996657078442</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
         <v>35.51886759690784</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>15.23141427681736</v>
       </c>
-      <c r="L6" t="n">
+      <c r="N6" t="n">
         <v>49.01838488091848</v>
       </c>
     </row>
@@ -705,33 +745,39 @@
         <v>3830938</v>
       </c>
       <c r="C7" t="n">
+        <v>2.973001204430317</v>
+      </c>
+      <c r="D7" t="n">
         <v>1855152</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
+        <v>3.084442488888936</v>
+      </c>
+      <c r="F7" t="n">
         <v>38.882714</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
         <v>1.9891</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>36.8056</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>36900</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>16886</v>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>45.76151761517615</v>
       </c>
-      <c r="J7" t="n">
+      <c r="L7" t="n">
         <v>8.641431440746388</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>36.22693664024569</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>52.60117959446765</v>
       </c>
     </row>
@@ -745,33 +791,39 @@
         <v>9310964</v>
       </c>
       <c r="C8" t="n">
+        <v>7.225777912983014</v>
+      </c>
+      <c r="D8" t="n">
         <v>4921131</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
+        <v>8.182049530059261</v>
+      </c>
+      <c r="F8" t="n">
         <v>41.498894</v>
       </c>
-      <c r="E8" t="n">
+      <c r="G8" t="n">
         <v>4.5306</v>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
         <v>45.8141</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>222957</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>140809</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>63.15522724112721</v>
       </c>
-      <c r="J8" t="n">
+      <c r="L8" t="n">
         <v>0.4632012352032939</v>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
         <v>14.97881943069797</v>
       </c>
-      <c r="L8" t="n">
+      <c r="N8" t="n">
         <v>84.0443116836456</v>
       </c>
     </row>
@@ -785,33 +837,39 @@
         <v>3279520</v>
       </c>
       <c r="C9" t="n">
+        <v>2.545073010827456</v>
+      </c>
+      <c r="D9" t="n">
         <v>1540535</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
+        <v>2.561348940475237</v>
+      </c>
+      <c r="F9" t="n">
         <v>39.179086</v>
       </c>
-      <c r="E9" t="n">
+      <c r="G9" t="n">
         <v>3.4147</v>
       </c>
-      <c r="F9" t="n">
+      <c r="H9" t="n">
         <v>34.1787</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>52604</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>22409</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>42.59942209717892</v>
       </c>
-      <c r="J9" t="n">
+      <c r="L9" t="n">
         <v>3.164998914600207</v>
       </c>
-      <c r="K9" t="n">
+      <c r="M9" t="n">
         <v>39.29597541821496</v>
       </c>
-      <c r="L9" t="n">
+      <c r="N9" t="n">
         <v>56.70740108244267</v>
       </c>
     </row>
@@ -825,33 +883,39 @@
         <v>763525</v>
       </c>
       <c r="C10" t="n">
+        <v>0.5925339289261945</v>
+      </c>
+      <c r="D10" t="n">
         <v>385344</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
+        <v>0.640686804336474</v>
+      </c>
+      <c r="F10" t="n">
         <v>38.955115</v>
       </c>
-      <c r="E10" t="n">
+      <c r="G10" t="n">
         <v>2.3576</v>
       </c>
-      <c r="F10" t="n">
+      <c r="H10" t="n">
         <v>46.8597</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>9085</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>3907</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>43.00495321959274</v>
       </c>
-      <c r="J10" t="n">
+      <c r="L10" t="n">
         <v>11.2863745451936</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>17.66017557055114</v>
       </c>
-      <c r="L10" t="n">
+      <c r="N10" t="n">
         <v>70.16310573301901</v>
       </c>
     </row>
@@ -865,33 +929,39 @@
         <v>1884857</v>
       </c>
       <c r="C11" t="n">
+        <v>1.462744145475315</v>
+      </c>
+      <c r="D11" t="n">
         <v>824826</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
+        <v>1.371385396097089</v>
+      </c>
+      <c r="F11" t="n">
         <v>39.153084</v>
       </c>
-      <c r="E11" t="n">
+      <c r="G11" t="n">
         <v>3.0872</v>
       </c>
-      <c r="F11" t="n">
+      <c r="H11" t="n">
         <v>49.4629</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>25464</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>13864</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>54.44549167452089</v>
       </c>
-      <c r="J11" t="n">
+      <c r="L11" t="n">
         <v>12.43516704571896</v>
       </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
         <v>27.23309339198011</v>
       </c>
-      <c r="L11" t="n">
+      <c r="N11" t="n">
         <v>59.65207252784095</v>
       </c>
     </row>
@@ -905,33 +975,39 @@
         <v>6303555</v>
       </c>
       <c r="C12" t="n">
+        <v>4.891876769395053</v>
+      </c>
+      <c r="D12" t="n">
         <v>2842643</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
+        <v>4.726280568892852</v>
+      </c>
+      <c r="F12" t="n">
         <v>38.892146</v>
       </c>
-      <c r="E12" t="n">
+      <c r="G12" t="n">
         <v>3.0708</v>
       </c>
-      <c r="F12" t="n">
+      <c r="H12" t="n">
         <v>54.6019</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>87292</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>34140</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>39.11011318333868</v>
       </c>
-      <c r="J12" t="n">
+      <c r="L12" t="n">
         <v>10.19532538685634</v>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>33.48604225015252</v>
       </c>
-      <c r="L12" t="n">
+      <c r="N12" t="n">
         <v>56.17414986330235</v>
       </c>
     </row>
@@ -945,33 +1021,39 @@
         <v>3589899</v>
       </c>
       <c r="C13" t="n">
+        <v>2.785942777143141</v>
+      </c>
+      <c r="D13" t="n">
         <v>1599844</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
+        <v>2.659958218622534</v>
+      </c>
+      <c r="F13" t="n">
         <v>40.664369</v>
       </c>
-      <c r="E13" t="n">
+      <c r="G13" t="n">
         <v>0.8064</v>
       </c>
-      <c r="F13" t="n">
+      <c r="H13" t="n">
         <v>78.98220000000001</v>
       </c>
-      <c r="G13" t="n">
+      <c r="I13" t="n">
         <v>12901</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>6858</v>
       </c>
-      <c r="I13" t="n">
+      <c r="K13" t="n">
         <v>53.15866987055266</v>
       </c>
-      <c r="J13" t="n">
+      <c r="L13" t="n">
         <v>33.98855535454015</v>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>16.13807175178945</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>49.73077167862992</v>
       </c>
     </row>
@@ -985,33 +1067,39 @@
         <v>3186741</v>
       </c>
       <c r="C14" t="n">
+        <v>2.47307182502235</v>
+      </c>
+      <c r="D14" t="n">
         <v>1483290</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
+        <v>2.466171343018831</v>
+      </c>
+      <c r="F14" t="n">
         <v>40.972066</v>
       </c>
-      <c r="E14" t="n">
+      <c r="G14" t="n">
         <v>2.2009</v>
       </c>
-      <c r="F14" t="n">
+      <c r="H14" t="n">
         <v>71.66379999999999</v>
       </c>
-      <c r="G14" t="n">
+      <c r="I14" t="n">
         <v>32645</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
         <v>19515</v>
       </c>
-      <c r="I14" t="n">
+      <c r="K14" t="n">
         <v>59.77944555062032</v>
       </c>
-      <c r="J14" t="n">
+      <c r="L14" t="n">
         <v>14.66147817005539</v>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>25.16122138772753</v>
       </c>
-      <c r="L14" t="n">
+      <c r="N14" t="n">
         <v>60.1276673479728</v>
       </c>
     </row>
@@ -1025,33 +1113,39 @@
         <v>8605534</v>
       </c>
       <c r="C15" t="n">
+        <v>6.678328635641203</v>
+      </c>
+      <c r="D15" t="n">
         <v>4164627</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
+        <v>6.924258750320224</v>
+      </c>
+      <c r="F15" t="n">
         <v>39.078355</v>
       </c>
-      <c r="E15" t="n">
+      <c r="G15" t="n">
         <v>2.3623</v>
       </c>
-      <c r="F15" t="n">
+      <c r="H15" t="n">
         <v>46.5578</v>
       </c>
-      <c r="G15" t="n">
+      <c r="I15" t="n">
         <v>98380</v>
       </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
         <v>39795</v>
       </c>
-      <c r="I15" t="n">
+      <c r="K15" t="n">
         <v>40.45029477536085</v>
       </c>
-      <c r="J15" t="n">
+      <c r="L15" t="n">
         <v>10.80544295513775</v>
       </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
         <v>27.16945133928165</v>
       </c>
-      <c r="L15" t="n">
+      <c r="N15" t="n">
         <v>61.57370666366307</v>
       </c>
     </row>
@@ -1065,33 +1159,39 @@
         <v>4930866</v>
       </c>
       <c r="C16" t="n">
+        <v>3.826600836892818</v>
+      </c>
+      <c r="D16" t="n">
         <v>2246319</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
+        <v>3.734810822616425</v>
+      </c>
+      <c r="F16" t="n">
         <v>39.828054</v>
       </c>
-      <c r="E16" t="n">
+      <c r="G16" t="n">
         <v>1.6685</v>
       </c>
-      <c r="F16" t="n">
+      <c r="H16" t="n">
         <v>66.85209999999999</v>
       </c>
-      <c r="G16" t="n">
+      <c r="I16" t="n">
         <v>37480</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
         <v>17153</v>
       </c>
-      <c r="I16" t="n">
+      <c r="K16" t="n">
         <v>45.76574172892209</v>
       </c>
-      <c r="J16" t="n">
+      <c r="L16" t="n">
         <v>22.71514583000391</v>
       </c>
-      <c r="K16" t="n">
+      <c r="M16" t="n">
         <v>21.02425753982069</v>
       </c>
-      <c r="L16" t="n">
+      <c r="N16" t="n">
         <v>56.20640526539054</v>
       </c>
     </row>
@@ -1105,33 +1205,39 @@
         <v>1985066</v>
       </c>
       <c r="C17" t="n">
+        <v>1.540511386212377</v>
+      </c>
+      <c r="D17" t="n">
         <v>883075</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
+        <v>1.468232280091118</v>
+      </c>
+      <c r="F17" t="n">
         <v>40.924809</v>
       </c>
-      <c r="E17" t="n">
+      <c r="G17" t="n">
         <v>2.726</v>
       </c>
-      <c r="F17" t="n">
+      <c r="H17" t="n">
         <v>64.1824</v>
       </c>
-      <c r="G17" t="n">
+      <c r="I17" t="n">
         <v>24073</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>12676</v>
       </c>
-      <c r="I17" t="n">
+      <c r="K17" t="n">
         <v>52.65650313629378</v>
       </c>
-      <c r="J17" t="n">
+      <c r="L17" t="n">
         <v>10.31336364758173</v>
       </c>
-      <c r="K17" t="n">
+      <c r="M17" t="n">
         <v>22.15198567640122</v>
       </c>
-      <c r="L17" t="n">
+      <c r="N17" t="n">
         <v>67.16887737164757</v>
       </c>
     </row>
@@ -1145,33 +1251,39 @@
         <v>17376320</v>
       </c>
       <c r="C18" t="n">
+        <v>13.48490116221317</v>
+      </c>
+      <c r="D18" t="n">
         <v>8217291</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
+        <v>13.66236378688358</v>
+      </c>
+      <c r="F18" t="n">
         <v>40.169901</v>
       </c>
-      <c r="E18" t="n">
+      <c r="G18" t="n">
         <v>4.4614</v>
       </c>
-      <c r="F18" t="n">
+      <c r="H18" t="n">
         <v>56.8465</v>
       </c>
-      <c r="G18" t="n">
+      <c r="I18" t="n">
         <v>366608</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>218067</v>
       </c>
-      <c r="I18" t="n">
+      <c r="K18" t="n">
         <v>59.48233535547506</v>
       </c>
-      <c r="J18" t="n">
+      <c r="L18" t="n">
         <v>3.852862228674881</v>
       </c>
-      <c r="K18" t="n">
+      <c r="M18" t="n">
         <v>24.98916336323859</v>
       </c>
-      <c r="L18" t="n">
+      <c r="N18" t="n">
         <v>70.82983735300483</v>
       </c>
     </row>
@@ -1185,33 +1297,39 @@
         <v>1248068</v>
       </c>
       <c r="C19" t="n">
+        <v>0.9685637478891427</v>
+      </c>
+      <c r="D19" t="n">
         <v>622716</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
+        <v>1.035350035420797</v>
+      </c>
+      <c r="F19" t="n">
         <v>39.71549</v>
       </c>
-      <c r="E19" t="n">
+      <c r="G19" t="n">
         <v>2.3804</v>
       </c>
-      <c r="F19" t="n">
+      <c r="H19" t="n">
         <v>59.71</v>
       </c>
-      <c r="G19" t="n">
+      <c r="I19" t="n">
         <v>14823</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
         <v>6852</v>
       </c>
-      <c r="I19" t="n">
+      <c r="K19" t="n">
         <v>46.2254604331107</v>
       </c>
-      <c r="J19" t="n">
+      <c r="L19" t="n">
         <v>16.89409155887632</v>
       </c>
-      <c r="K19" t="n">
+      <c r="M19" t="n">
         <v>16.63615142796512</v>
       </c>
-      <c r="L19" t="n">
+      <c r="N19" t="n">
         <v>65.42055921025576</v>
       </c>
     </row>
@@ -1225,33 +1343,39 @@
         <v>6009420</v>
       </c>
       <c r="C20" t="n">
+        <v>4.663613166782557</v>
+      </c>
+      <c r="D20" t="n">
         <v>2919303</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
+        <v>4.853738244165943</v>
+      </c>
+      <c r="F20" t="n">
         <v>39.421559</v>
       </c>
-      <c r="E20" t="n">
+      <c r="G20" t="n">
         <v>3.5718</v>
       </c>
-      <c r="F20" t="n">
+      <c r="H20" t="n">
         <v>35.7643</v>
       </c>
-      <c r="G20" t="n">
+      <c r="I20" t="n">
         <v>104272</v>
       </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
         <v>36716</v>
       </c>
-      <c r="I20" t="n">
+      <c r="K20" t="n">
         <v>35.21175387448212</v>
       </c>
-      <c r="J20" t="n">
+      <c r="L20" t="n">
         <v>2.396954065514731</v>
       </c>
-      <c r="K20" t="n">
+      <c r="M20" t="n">
         <v>31.89900928266864</v>
       </c>
-      <c r="L20" t="n">
+      <c r="N20" t="n">
         <v>65.29249589080902</v>
       </c>
     </row>
@@ -1265,33 +1389,39 @@
         <v>4222400</v>
       </c>
       <c r="C21" t="n">
+        <v>3.276795470348664</v>
+      </c>
+      <c r="D21" t="n">
         <v>1930924</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
+        <v>3.210423743399668</v>
+      </c>
+      <c r="F21" t="n">
         <v>41.805956</v>
       </c>
-      <c r="E21" t="n">
+      <c r="G21" t="n">
         <v>1.2834</v>
       </c>
-      <c r="F21" t="n">
+      <c r="H21" t="n">
         <v>81.2405</v>
       </c>
-      <c r="G21" t="n">
+      <c r="I21" t="n">
         <v>24781</v>
       </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
         <v>14379</v>
       </c>
-      <c r="I21" t="n">
+      <c r="K21" t="n">
         <v>58.02429280497156</v>
       </c>
-      <c r="J21" t="n">
+      <c r="L21" t="n">
         <v>30.11584125640102</v>
       </c>
-      <c r="K21" t="n">
+      <c r="M21" t="n">
         <v>20.20771788895167</v>
       </c>
-      <c r="L21" t="n">
+      <c r="N21" t="n">
         <v>49.65204604271558</v>
       </c>
     </row>
@@ -1305,33 +1435,39 @@
         <v>6668557</v>
       </c>
       <c r="C22" t="n">
+        <v>5.175136740091387</v>
+      </c>
+      <c r="D22" t="n">
         <v>3016552</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
+        <v>5.015427931912263</v>
+      </c>
+      <c r="F22" t="n">
         <v>39.416127</v>
       </c>
-      <c r="E22" t="n">
+      <c r="G22" t="n">
         <v>2.7928</v>
       </c>
-      <c r="F22" t="n">
+      <c r="H22" t="n">
         <v>71.25069999999999</v>
       </c>
-      <c r="G22" t="n">
+      <c r="I22" t="n">
         <v>84247</v>
       </c>
-      <c r="H22" t="n">
+      <c r="J22" t="n">
         <v>56164</v>
       </c>
-      <c r="I22" t="n">
+      <c r="K22" t="n">
         <v>66.66587534274217</v>
       </c>
-      <c r="J22" t="n">
+      <c r="L22" t="n">
         <v>19.08010933378349</v>
       </c>
-      <c r="K22" t="n">
+      <c r="M22" t="n">
         <v>25.79908979454729</v>
       </c>
-      <c r="L22" t="n">
+      <c r="N22" t="n">
         <v>54.89217526826165</v>
       </c>
     </row>
@@ -1345,33 +1481,39 @@
         <v>2461932</v>
       </c>
       <c r="C23" t="n">
+        <v>1.910583465779279</v>
+      </c>
+      <c r="D23" t="n">
         <v>1111103</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
+        <v>1.84735984045079</v>
+      </c>
+      <c r="F23" t="n">
         <v>38.926068</v>
       </c>
-      <c r="E23" t="n">
+      <c r="G23" t="n">
         <v>3.6262</v>
       </c>
-      <c r="F23" t="n">
+      <c r="H23" t="n">
         <v>42.7057</v>
       </c>
-      <c r="G23" t="n">
+      <c r="I23" t="n">
         <v>40291</v>
       </c>
-      <c r="H23" t="n">
+      <c r="J23" t="n">
         <v>21662</v>
       </c>
-      <c r="I23" t="n">
+      <c r="K23" t="n">
         <v>53.76386786130898</v>
       </c>
-      <c r="J23" t="n">
+      <c r="L23" t="n">
         <v>4.621259380731631</v>
       </c>
-      <c r="K23" t="n">
+      <c r="M23" t="n">
         <v>33.59011665913344</v>
       </c>
-      <c r="L23" t="n">
+      <c r="N23" t="n">
         <v>61.63042625596277</v>
       </c>
     </row>
@@ -1385,33 +1527,39 @@
         <v>1936873</v>
       </c>
       <c r="C24" t="n">
+        <v>1.503111186301778</v>
+      </c>
+      <c r="D24" t="n">
         <v>987173</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
+        <v>1.641309361757936</v>
+      </c>
+      <c r="F24" t="n">
         <v>38.864663</v>
       </c>
-      <c r="E24" t="n">
+      <c r="G24" t="n">
         <v>1.9719</v>
       </c>
-      <c r="F24" t="n">
+      <c r="H24" t="n">
         <v>46.7041</v>
       </c>
-      <c r="G24" t="n">
+      <c r="I24" t="n">
         <v>19466</v>
       </c>
-      <c r="H24" t="n">
+      <c r="J24" t="n">
         <v>11412</v>
       </c>
-      <c r="I24" t="n">
+      <c r="K24" t="n">
         <v>58.62529538682831</v>
       </c>
-      <c r="J24" t="n">
+      <c r="L24" t="n">
         <v>4.250253434148973</v>
       </c>
-      <c r="K24" t="n">
+      <c r="M24" t="n">
         <v>15.92744498076381</v>
       </c>
-      <c r="L24" t="n">
+      <c r="N24" t="n">
         <v>79.73312169902667</v>
       </c>
     </row>
@@ -1425,33 +1573,39 @@
         <v>2852489</v>
       </c>
       <c r="C25" t="n">
+        <v>2.213675406029602</v>
+      </c>
+      <c r="D25" t="n">
         <v>1306723</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
+        <v>2.172604693528303</v>
+      </c>
+      <c r="F25" t="n">
         <v>40.135747</v>
       </c>
-      <c r="E25" t="n">
+      <c r="G25" t="n">
         <v>2.7125</v>
       </c>
-      <c r="F25" t="n">
+      <c r="H25" t="n">
         <v>54.4891</v>
       </c>
-      <c r="G25" t="n">
+      <c r="I25" t="n">
         <v>35445</v>
       </c>
-      <c r="H25" t="n">
+      <c r="J25" t="n">
         <v>14655</v>
       </c>
-      <c r="I25" t="n">
+      <c r="K25" t="n">
         <v>41.34574693186627</v>
       </c>
-      <c r="J25" t="n">
+      <c r="L25" t="n">
         <v>13.78699230223444</v>
       </c>
-      <c r="K25" t="n">
+      <c r="M25" t="n">
         <v>30.19174405598146</v>
       </c>
-      <c r="L25" t="n">
+      <c r="N25" t="n">
         <v>55.49604413826087</v>
       </c>
     </row>
@@ -1465,33 +1619,39 @@
         <v>3068972</v>
       </c>
       <c r="C26" t="n">
+        <v>2.381677138174233</v>
+      </c>
+      <c r="D26" t="n">
         <v>1466293</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
+        <v>2.437911519034788</v>
+      </c>
+      <c r="F26" t="n">
         <v>40.402563</v>
       </c>
-      <c r="E26" t="n">
+      <c r="G26" t="n">
         <v>2.7863</v>
       </c>
-      <c r="F26" t="n">
+      <c r="H26" t="n">
         <v>46.3876</v>
       </c>
-      <c r="G26" t="n">
+      <c r="I26" t="n">
         <v>40855</v>
       </c>
-      <c r="H26" t="n">
+      <c r="J26" t="n">
         <v>24318</v>
       </c>
-      <c r="I26" t="n">
+      <c r="K26" t="n">
         <v>59.52270223962795</v>
       </c>
-      <c r="J26" t="n">
+      <c r="L26" t="n">
         <v>13.90639228082877</v>
       </c>
-      <c r="K26" t="n">
+      <c r="M26" t="n">
         <v>20.75811084031715</v>
       </c>
-      <c r="L26" t="n">
+      <c r="N26" t="n">
         <v>64.73596185874096</v>
       </c>
     </row>
@@ -1505,33 +1665,39 @@
         <v>3000220</v>
       </c>
       <c r="C27" t="n">
+        <v>2.328322116817324</v>
+      </c>
+      <c r="D27" t="n">
         <v>1445570</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
+        <v>2.403456713338411</v>
+      </c>
+      <c r="F27" t="n">
         <v>39.47098</v>
       </c>
-      <c r="E27" t="n">
+      <c r="G27" t="n">
         <v>2.5479</v>
       </c>
-      <c r="F27" t="n">
+      <c r="H27" t="n">
         <v>42.3213</v>
       </c>
-      <c r="G27" t="n">
+      <c r="I27" t="n">
         <v>36831</v>
       </c>
-      <c r="H27" t="n">
+      <c r="J27" t="n">
         <v>19168</v>
       </c>
-      <c r="I27" t="n">
+      <c r="K27" t="n">
         <v>52.04311585349298</v>
       </c>
-      <c r="J27" t="n">
+      <c r="L27" t="n">
         <v>9.867832153436513</v>
       </c>
-      <c r="K27" t="n">
+      <c r="M27" t="n">
         <v>29.42014099134048</v>
       </c>
-      <c r="L27" t="n">
+      <c r="N27" t="n">
         <v>59.30828918628646</v>
       </c>
     </row>
@@ -1545,33 +1711,39 @@
         <v>2467247</v>
       </c>
       <c r="C28" t="n">
+        <v>1.914708173984305</v>
+      </c>
+      <c r="D28" t="n">
         <v>1089415</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
+        <v>1.811300591020542</v>
+      </c>
+      <c r="F28" t="n">
         <v>39.908913</v>
       </c>
-      <c r="E28" t="n">
+      <c r="G28" t="n">
         <v>4.1814</v>
       </c>
-      <c r="F28" t="n">
+      <c r="H28" t="n">
         <v>63.683</v>
       </c>
-      <c r="G28" t="n">
+      <c r="I28" t="n">
         <v>45553</v>
       </c>
-      <c r="H28" t="n">
+      <c r="J28" t="n">
         <v>26357</v>
       </c>
-      <c r="I28" t="n">
+      <c r="K28" t="n">
         <v>57.86007507738239</v>
       </c>
-      <c r="J28" t="n">
+      <c r="L28" t="n">
         <v>14.21730075431427</v>
       </c>
-      <c r="K28" t="n">
+      <c r="M28" t="n">
         <v>22.06000410015884</v>
       </c>
-      <c r="L28" t="n">
+      <c r="N28" t="n">
         <v>63.40407065301735</v>
       </c>
     </row>
@@ -1585,33 +1757,39 @@
         <v>3589293</v>
       </c>
       <c r="C29" t="n">
+        <v>2.785472490563226</v>
+      </c>
+      <c r="D29" t="n">
         <v>1672565</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
+        <v>2.780866770716644</v>
+      </c>
+      <c r="F29" t="n">
         <v>40.393153</v>
       </c>
-      <c r="E29" t="n">
+      <c r="G29" t="n">
         <v>3.1207</v>
       </c>
-      <c r="F29" t="n">
+      <c r="H29" t="n">
         <v>44.7446</v>
       </c>
-      <c r="G29" t="n">
+      <c r="I29" t="n">
         <v>52196</v>
       </c>
-      <c r="H29" t="n">
+      <c r="J29" t="n">
         <v>33408</v>
       </c>
-      <c r="I29" t="n">
+      <c r="K29" t="n">
         <v>64.00490459039007</v>
       </c>
-      <c r="J29" t="n">
+      <c r="L29" t="n">
         <v>5.374825116994955</v>
       </c>
-      <c r="K29" t="n">
+      <c r="M29" t="n">
         <v>30.44244860275654</v>
       </c>
-      <c r="L29" t="n">
+      <c r="N29" t="n">
         <v>62.56432948297579</v>
       </c>
     </row>
@@ -1625,33 +1803,39 @@
         <v>1402979</v>
       </c>
       <c r="C30" t="n">
+        <v>1.088782500993345</v>
+      </c>
+      <c r="D30" t="n">
         <v>648539</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
+        <v>1.078284284684782</v>
+      </c>
+      <c r="F30" t="n">
         <v>39.55807</v>
       </c>
-      <c r="E30" t="n">
+      <c r="G30" t="n">
         <v>3.3307</v>
       </c>
-      <c r="F30" t="n">
+      <c r="H30" t="n">
         <v>69.7855</v>
       </c>
-      <c r="G30" t="n">
+      <c r="I30" t="n">
         <v>21601</v>
       </c>
-      <c r="H30" t="n">
+      <c r="J30" t="n">
         <v>13826</v>
       </c>
-      <c r="I30" t="n">
+      <c r="K30" t="n">
         <v>64.00629600481459</v>
       </c>
-      <c r="J30" t="n">
+      <c r="L30" t="n">
         <v>10.08648383093703</v>
       </c>
-      <c r="K30" t="n">
+      <c r="M30" t="n">
         <v>36.32288998274151</v>
       </c>
-      <c r="L30" t="n">
+      <c r="N30" t="n">
         <v>53.18229234788767</v>
       </c>
     </row>
@@ -1665,33 +1849,39 @@
         <v>8150203</v>
       </c>
       <c r="C31" t="n">
+        <v>6.324968802771432</v>
+      </c>
+      <c r="D31" t="n">
         <v>3428792</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
+        <v>5.700832993933906</v>
+      </c>
+      <c r="F31" t="n">
         <v>41.889429</v>
       </c>
-      <c r="E31" t="n">
+      <c r="G31" t="n">
         <v>2.3531</v>
       </c>
-      <c r="F31" t="n">
+      <c r="H31" t="n">
         <v>67.2895</v>
       </c>
-      <c r="G31" t="n">
+      <c r="I31" t="n">
         <v>80682</v>
       </c>
-      <c r="H31" t="n">
+      <c r="J31" t="n">
         <v>60696</v>
       </c>
-      <c r="I31" t="n">
+      <c r="K31" t="n">
         <v>75.22867554101286</v>
       </c>
-      <c r="J31" t="n">
+      <c r="L31" t="n">
         <v>21.42952292487404</v>
       </c>
-      <c r="K31" t="n">
+      <c r="M31" t="n">
         <v>17.07425980627876</v>
       </c>
-      <c r="L31" t="n">
+      <c r="N31" t="n">
         <v>61.0801915110316</v>
       </c>
     </row>
@@ -1705,33 +1895,39 @@
         <v>2368695</v>
       </c>
       <c r="C32" t="n">
+        <v>1.838226848862621</v>
+      </c>
+      <c r="D32" t="n">
         <v>1241444</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
+        <v>2.064069478498924</v>
+      </c>
+      <c r="F32" t="n">
         <v>39.567117</v>
       </c>
-      <c r="E32" t="n">
+      <c r="G32" t="n">
         <v>1.9883</v>
       </c>
-      <c r="F32" t="n">
+      <c r="H32" t="n">
         <v>60.4067</v>
       </c>
-      <c r="G32" t="n">
+      <c r="I32" t="n">
         <v>24684</v>
       </c>
-      <c r="H32" t="n">
+      <c r="J32" t="n">
         <v>11567</v>
       </c>
-      <c r="I32" t="n">
+      <c r="K32" t="n">
         <v>46.86031437368336</v>
       </c>
-      <c r="J32" t="n">
+      <c r="L32" t="n">
         <v>8.245175712548077</v>
       </c>
-      <c r="K32" t="n">
+      <c r="M32" t="n">
         <v>26.56201716032743</v>
       </c>
-      <c r="L32" t="n">
+      <c r="N32" t="n">
         <v>65.05572175285184</v>
       </c>
     </row>
@@ -1745,33 +1941,39 @@
         <v>1635256</v>
       </c>
       <c r="C33" t="n">
+        <v>1.269041174133307</v>
+      </c>
+      <c r="D33" t="n">
         <v>692465</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
+        <v>1.151317233341784</v>
+      </c>
+      <c r="F33" t="n">
         <v>40.029822</v>
       </c>
-      <c r="E33" t="n">
+      <c r="G33" t="n">
         <v>2.36</v>
       </c>
-      <c r="F33" t="n">
+      <c r="H33" t="n">
         <v>62.3801</v>
       </c>
-      <c r="G33" t="n">
+      <c r="I33" t="n">
         <v>16342</v>
       </c>
-      <c r="H33" t="n">
+      <c r="J33" t="n">
         <v>7647</v>
       </c>
-      <c r="I33" t="n">
+      <c r="K33" t="n">
         <v>46.79353812262881</v>
       </c>
-      <c r="J33" t="n">
+      <c r="L33" t="n">
         <v>23.84699233719309</v>
       </c>
-      <c r="K33" t="n">
+      <c r="M33" t="n">
         <v>23.2657371513763</v>
       </c>
-      <c r="L33" t="n">
+      <c r="N33" t="n">
         <v>52.46855971472646</v>
       </c>
     </row>

</xml_diff>